<commit_message>
Creación de datasets finales
</commit_message>
<xml_diff>
--- a/fuentes_datos/datasets_finales/escuela.xlsx
+++ b/fuentes_datos/datasets_finales/escuela.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carolina\Documents\Proyectos_programacion\MD_Datos_sinteticos_repitencias\datasets_finales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carolina\Documents\Proyectos_programacion\PredEstu\fuentes_datos\datasets_finales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32B0C68-C4CE-4A28-8669-2E080FB8B965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2470F734-CD62-46CD-8034-6D0A513D40CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>id_escuela</t>
   </si>
   <si>
     <t>nombre</t>
+  </si>
+  <si>
+    <t>Ingeniería de Sistemas</t>
+  </si>
+  <si>
+    <t>Ingeniería de Software</t>
+  </si>
+  <si>
+    <t>Ciencias de la Computación</t>
   </si>
 </sst>
 </file>
@@ -351,7 +360,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -372,15 +381,24 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>